<commit_message>
learning sensitivity failure 機能実装
</commit_message>
<xml_diff>
--- a/プロトタイプ資料.xlsx
+++ b/プロトタイプ資料.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="外部機能一覧" sheetId="1" r:id="rId1"/>
     <sheet name="内部機能クラス一覧" sheetId="2" r:id="rId2"/>
-    <sheet name="アプリケーションエラーメッセージ一覧" sheetId="3" r:id="rId3"/>
+    <sheet name="アプリケーションメッセージ一覧" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="175">
   <si>
     <t>機能名</t>
     <rPh sb="0" eb="3">
@@ -709,15 +709,424 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>メッセージ文</t>
-    <rPh sb="5" eb="6">
+    <t>Settings</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>__init__</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>information</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>instantized</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>debug</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>__check_settings_format</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>critical</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>error</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>wav_directory:指定パスは存在しません[入力値]</t>
+    <rPh sb="19" eb="21">
+      <t>ソンザイ</t>
+    </rPh>
+    <rPh sb="26" eb="28">
+      <t>ニュウリョク</t>
+    </rPh>
+    <rPh sb="28" eb="29">
+      <t>アタイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>chart_save_directory:指定パスは存在しません。分析画像出力を無効化しました[入力値]</t>
+    <rPh sb="48" eb="50">
+      <t>ニュウリョク</t>
+    </rPh>
+    <rPh sb="50" eb="51">
+      <t>アタイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>アプリケーション設定ファイルロード成功</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>アプリケーション設定パラメータフォーマットチェック完了</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>測定局別設定パラメータフォーマットチェック完了</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>__check_signal_process_settings_format</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>critical</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>critical</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>log_save_directory:指定パスは存在しません[入力値]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>signal_process_settings:tapは2のべき乗の整数を指定して下さい[入力値]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>signal_process_settings:overlap_rateは0.0から0.99の範囲で指定して下さい[入力値]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>signal_process_settings:window-窓関数の入力値が無効[入力値]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>signal_process_settings:mean_timeは0.1から3.0の範囲で指定して下さい[入力値]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>__check_detector_common_settings_format</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>__check_detector_common_settings_format</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>__check_detector_common_settings_format</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>detector_common_settings:system_start_dateの入力値不正[エラー文]</t>
+    <rPh sb="52" eb="53">
       <t>ブン</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>メソッド</t>
-    <phoneticPr fontId="1"/>
+    <t>detector_common_settings:common_calibrated_timeの入力値不正[エラー文]</t>
+    <rPh sb="57" eb="58">
+      <t>ブン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>__check_station_settings</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>__check_station_settings</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>__check_station_settings</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>__check_station_settings</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>__check_station_settings</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>station_settings:設定ファイル内でstationidが重複しています[設定ファイル内の測定局IDリスト]</t>
+    <rPh sb="43" eb="45">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="49" eb="50">
+      <t>ナイ</t>
+    </rPh>
+    <rPh sb="51" eb="54">
+      <t>ソクテイキョク</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>detector_common_settings:valid_common_calibrated_timeはtrueもしくはfalseで指定して下さい[入力値]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>detector_common_settings:system_start_dateは現在日より後には設定できません[入力値]</t>
+    <rPh sb="59" eb="61">
+      <t>ニュウリョク</t>
+    </rPh>
+    <rPh sb="61" eb="62">
+      <t>アタイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>detector_common_settings:return_daysは1から100までの整数で指定して下さい[入力値]</t>
+    <rPh sb="57" eb="60">
+      <t>ニュウリョクアタイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>station_settings:stationidの文字数不正[入力値]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>station_settings:{測定局ID}:learnig_validはtrueもしくはfalseで指定して下さい[入力値]</t>
+    <rPh sb="18" eb="21">
+      <t>ソクテイキョク</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>station_settings:{測定局ID}:internal_cal_levelの入力値不正[入力値]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>station_settings:{測定局ID}:sensitivity_target_freqencyの入力値不正[入力値]
+利用可能な周波数一覧:{AVAILABLE_FREQS}</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>station_settings:{測定局ID}:sensitivity_validはtrueもしくはfalseで指定して下さい[入力値]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>station_settings:{測定局ID}:sensitivity_toleranceは0.0から1.0までの範囲で指定して下さい[入力値]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>station_settings:{測定局ID}:failure_validはtrueもしくはfalseで指定して下さい[入力値]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>station_settings:{測定局ID}:failure_target_freqencyの入力値不正[入力値]
+利用可能な周波数一覧:{AVAILABLE_FREQS}</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>station_settings:{測定局ID}:failure_toleranceは0.0から10.0までの範囲で指定して下さい[入力値]</t>
+    <rPh sb="66" eb="69">
+      <t>ニュウリョクアタイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>出力クラス</t>
+    <rPh sb="0" eb="2">
+      <t>シュツリョク</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>出力メソッド</t>
+    <rPh sb="0" eb="2">
+      <t>シュツリョク</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>メッセージ</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>station_settings:{測定局ID}:calibrated_timeは現在時刻より後には設定できません[入力値]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>station_settings:{{測定局ID}:calibrated_timeの入力値不正[エラー文]</t>
+    <rPh sb="51" eb="52">
+      <t>ブン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>detector_common_settings:common_calibrated_timeは現在時刻より後には設定できません[入力値]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>detector_common_settings:learning_sample_sizeは385から1000までの整数で指定して下さい[入力値]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>detector_common_settings:sensitivity_confidence_levelは0.9から0.99までの範囲で指定して下さい[入力値]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>detector_common_settings:sensitivity_sample_sizeは30から1000までの整数で指定して下さい[入力値]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>detector_common_settings:sensitivity_reload_limit_sizeは0から0.5までの範囲で指定して下さい[入力値]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>detector_common_settings:sensitivity_peak_level_percentileは1から100までの範囲で指定して下さい[入力値]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>detector_common_settings:valid_sensitivity_save_chartはtrueもしくはfalseで指定して下さい[入力値]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>detector_common_settings:failure_confidence_levelは0.9から0.99までの範囲で指定して下さい[入力値]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>detector_common_settings:failure_floor_level_percentileは1から100までの範囲で指定して下さい[入力値]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>detector_common_settings:learning_target_freqsの入力値不正[入力値]
+利用可能な周波数一覧:{VAILABLE_FREQS}</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>WindowsEventLogger</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>EventID</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>002</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>001</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>003</t>
+  </si>
+  <si>
+    <t>004</t>
+  </si>
+  <si>
+    <t>005</t>
+  </si>
+  <si>
+    <t>006</t>
+  </si>
+  <si>
+    <t>007</t>
+  </si>
+  <si>
+    <t>008</t>
+  </si>
+  <si>
+    <t>009</t>
+  </si>
+  <si>
+    <t>010</t>
+  </si>
+  <si>
+    <t>011</t>
+  </si>
+  <si>
+    <t>012</t>
+  </si>
+  <si>
+    <t>013</t>
+  </si>
+  <si>
+    <t>014</t>
+  </si>
+  <si>
+    <t>015</t>
+  </si>
+  <si>
+    <t>016</t>
+  </si>
+  <si>
+    <t>017</t>
+  </si>
+  <si>
+    <t>018</t>
+  </si>
+  <si>
+    <t>019</t>
+  </si>
+  <si>
+    <t>020</t>
+  </si>
+  <si>
+    <t>021</t>
+  </si>
+  <si>
+    <t>022</t>
+  </si>
+  <si>
+    <t>023</t>
+  </si>
+  <si>
+    <t>024</t>
+  </si>
+  <si>
+    <t>025</t>
+  </si>
+  <si>
+    <t>026</t>
+  </si>
+  <si>
+    <t>027</t>
+  </si>
+  <si>
+    <t>028</t>
+  </si>
+  <si>
+    <t>029</t>
+  </si>
+  <si>
+    <t>030</t>
+  </si>
+  <si>
+    <t>031</t>
+  </si>
+  <si>
+    <t>032</t>
+  </si>
+  <si>
+    <t>033</t>
+  </si>
+  <si>
+    <t>034</t>
+  </si>
+  <si>
+    <t>035</t>
+  </si>
+  <si>
+    <t>036</t>
+  </si>
+  <si>
+    <t>037</t>
+  </si>
+  <si>
+    <t>038</t>
+  </si>
+  <si>
+    <t>039</t>
   </si>
 </sst>
 </file>
@@ -818,7 +1227,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -847,6 +1256,12 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1539,36 +1954,707 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:E40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="18.6640625" customWidth="1"/>
-    <col min="2" max="2" width="14.75" customWidth="1"/>
-    <col min="3" max="3" width="23" customWidth="1"/>
-    <col min="4" max="4" width="27.1640625" customWidth="1"/>
+    <col min="1" max="1" width="8.6640625" style="11"/>
+    <col min="2" max="2" width="21" customWidth="1"/>
+    <col min="3" max="3" width="40.08203125" customWidth="1"/>
+    <col min="4" max="4" width="11.9140625" customWidth="1"/>
+    <col min="5" max="5" width="97.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" t="s">
-        <v>2</v>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="11" t="s">
+        <v>135</v>
       </c>
       <c r="B1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="B2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C2" t="s">
         <v>76</v>
       </c>
-      <c r="C1" t="s">
-        <v>74</v>
-      </c>
-      <c r="D1" t="s">
-        <v>75</v>
+      <c r="D2" t="s">
+        <v>77</v>
+      </c>
+      <c r="E2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="B3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C3" t="s">
+        <v>76</v>
+      </c>
+      <c r="D3" t="s">
+        <v>77</v>
+      </c>
+      <c r="E3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="B4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C4" t="s">
+        <v>76</v>
+      </c>
+      <c r="D4" t="s">
+        <v>77</v>
+      </c>
+      <c r="E4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="B5" t="s">
+        <v>75</v>
+      </c>
+      <c r="C5" t="s">
+        <v>76</v>
+      </c>
+      <c r="D5" t="s">
+        <v>79</v>
+      </c>
+      <c r="E5" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="11" t="s">
+        <v>140</v>
+      </c>
+      <c r="B6" t="s">
+        <v>75</v>
+      </c>
+      <c r="C6" t="s">
+        <v>80</v>
+      </c>
+      <c r="D6" t="s">
+        <v>81</v>
+      </c>
+      <c r="E6" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="B7" t="s">
+        <v>75</v>
+      </c>
+      <c r="C7" t="s">
+        <v>80</v>
+      </c>
+      <c r="D7" t="s">
+        <v>81</v>
+      </c>
+      <c r="E7" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="B8" t="s">
+        <v>75</v>
+      </c>
+      <c r="C8" t="s">
+        <v>80</v>
+      </c>
+      <c r="D8" t="s">
+        <v>82</v>
+      </c>
+      <c r="E8" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="11" t="s">
+        <v>143</v>
+      </c>
+      <c r="B9" t="s">
+        <v>75</v>
+      </c>
+      <c r="C9" t="s">
+        <v>88</v>
+      </c>
+      <c r="D9" t="s">
+        <v>89</v>
+      </c>
+      <c r="E9" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="B10" t="s">
+        <v>75</v>
+      </c>
+      <c r="C10" t="s">
+        <v>88</v>
+      </c>
+      <c r="D10" t="s">
+        <v>89</v>
+      </c>
+      <c r="E10" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="B11" t="s">
+        <v>75</v>
+      </c>
+      <c r="C11" t="s">
+        <v>88</v>
+      </c>
+      <c r="D11" t="s">
+        <v>90</v>
+      </c>
+      <c r="E11" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="B12" t="s">
+        <v>75</v>
+      </c>
+      <c r="C12" t="s">
+        <v>88</v>
+      </c>
+      <c r="D12" t="s">
+        <v>90</v>
+      </c>
+      <c r="E12" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="B13" t="s">
+        <v>75</v>
+      </c>
+      <c r="C13" t="s">
+        <v>96</v>
+      </c>
+      <c r="D13" t="s">
+        <v>90</v>
+      </c>
+      <c r="E13" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="B14" t="s">
+        <v>75</v>
+      </c>
+      <c r="C14" t="s">
+        <v>97</v>
+      </c>
+      <c r="D14" t="s">
+        <v>90</v>
+      </c>
+      <c r="E14" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" s="11" t="s">
+        <v>149</v>
+      </c>
+      <c r="B15" t="s">
+        <v>75</v>
+      </c>
+      <c r="C15" t="s">
+        <v>98</v>
+      </c>
+      <c r="D15" t="s">
+        <v>90</v>
+      </c>
+      <c r="E15" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="B16" t="s">
+        <v>75</v>
+      </c>
+      <c r="C16" t="s">
+        <v>98</v>
+      </c>
+      <c r="D16" t="s">
+        <v>90</v>
+      </c>
+      <c r="E16" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="B17" t="s">
+        <v>75</v>
+      </c>
+      <c r="C17" t="s">
+        <v>96</v>
+      </c>
+      <c r="D17" t="s">
+        <v>90</v>
+      </c>
+      <c r="E17" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" s="11" t="s">
+        <v>152</v>
+      </c>
+      <c r="B18" t="s">
+        <v>75</v>
+      </c>
+      <c r="C18" t="s">
+        <v>96</v>
+      </c>
+      <c r="D18" t="s">
+        <v>90</v>
+      </c>
+      <c r="E18" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="B19" t="s">
+        <v>75</v>
+      </c>
+      <c r="C19" t="s">
+        <v>98</v>
+      </c>
+      <c r="D19" t="s">
+        <v>90</v>
+      </c>
+      <c r="E19" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="36" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="B20" t="s">
+        <v>75</v>
+      </c>
+      <c r="C20" t="s">
+        <v>98</v>
+      </c>
+      <c r="D20" t="s">
+        <v>90</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21" s="11" t="s">
+        <v>155</v>
+      </c>
+      <c r="B21" t="s">
+        <v>75</v>
+      </c>
+      <c r="C21" t="s">
+        <v>96</v>
+      </c>
+      <c r="D21" t="s">
+        <v>90</v>
+      </c>
+      <c r="E21" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="B22" t="s">
+        <v>75</v>
+      </c>
+      <c r="C22" t="s">
+        <v>96</v>
+      </c>
+      <c r="D22" t="s">
+        <v>90</v>
+      </c>
+      <c r="E22" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="B23" t="s">
+        <v>75</v>
+      </c>
+      <c r="C23" t="s">
+        <v>98</v>
+      </c>
+      <c r="D23" t="s">
+        <v>90</v>
+      </c>
+      <c r="E23" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="B24" t="s">
+        <v>75</v>
+      </c>
+      <c r="C24" t="s">
+        <v>98</v>
+      </c>
+      <c r="D24" t="s">
+        <v>90</v>
+      </c>
+      <c r="E24" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A25" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="B25" t="s">
+        <v>75</v>
+      </c>
+      <c r="C25" t="s">
+        <v>96</v>
+      </c>
+      <c r="D25" t="s">
+        <v>90</v>
+      </c>
+      <c r="E25" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26" s="11" t="s">
+        <v>160</v>
+      </c>
+      <c r="B26" t="s">
+        <v>75</v>
+      </c>
+      <c r="C26" t="s">
+        <v>96</v>
+      </c>
+      <c r="D26" t="s">
+        <v>90</v>
+      </c>
+      <c r="E26" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A27" s="11" t="s">
+        <v>161</v>
+      </c>
+      <c r="B27" t="s">
+        <v>75</v>
+      </c>
+      <c r="C27" t="s">
+        <v>96</v>
+      </c>
+      <c r="D27" t="s">
+        <v>90</v>
+      </c>
+      <c r="E27" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A28" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="B28" t="s">
+        <v>75</v>
+      </c>
+      <c r="C28" t="s">
+        <v>101</v>
+      </c>
+      <c r="D28" t="s">
+        <v>90</v>
+      </c>
+      <c r="E28" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A29" s="11" t="s">
+        <v>163</v>
+      </c>
+      <c r="B29" t="s">
+        <v>75</v>
+      </c>
+      <c r="C29" t="s">
+        <v>102</v>
+      </c>
+      <c r="D29" t="s">
+        <v>90</v>
+      </c>
+      <c r="E29" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A30" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="B30" t="s">
+        <v>75</v>
+      </c>
+      <c r="C30" t="s">
+        <v>103</v>
+      </c>
+      <c r="D30" t="s">
+        <v>90</v>
+      </c>
+      <c r="E30" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A31" s="11" t="s">
+        <v>165</v>
+      </c>
+      <c r="B31" t="s">
+        <v>75</v>
+      </c>
+      <c r="C31" t="s">
+        <v>104</v>
+      </c>
+      <c r="D31" t="s">
+        <v>90</v>
+      </c>
+      <c r="E31" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A32" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="B32" t="s">
+        <v>75</v>
+      </c>
+      <c r="C32" t="s">
+        <v>104</v>
+      </c>
+      <c r="D32" t="s">
+        <v>90</v>
+      </c>
+      <c r="E32" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A33" s="11" t="s">
+        <v>167</v>
+      </c>
+      <c r="B33" t="s">
+        <v>75</v>
+      </c>
+      <c r="C33" t="s">
+        <v>105</v>
+      </c>
+      <c r="D33" t="s">
+        <v>90</v>
+      </c>
+      <c r="E33" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A34" s="11" t="s">
+        <v>168</v>
+      </c>
+      <c r="B34" t="s">
+        <v>75</v>
+      </c>
+      <c r="C34" t="s">
+        <v>101</v>
+      </c>
+      <c r="D34" t="s">
+        <v>90</v>
+      </c>
+      <c r="E34" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="36" x14ac:dyDescent="0.55000000000000004">
+      <c r="A35" s="11" t="s">
+        <v>169</v>
+      </c>
+      <c r="B35" t="s">
+        <v>75</v>
+      </c>
+      <c r="C35" t="s">
+        <v>102</v>
+      </c>
+      <c r="D35" t="s">
+        <v>90</v>
+      </c>
+      <c r="E35" s="10" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A36" s="11" t="s">
+        <v>170</v>
+      </c>
+      <c r="B36" t="s">
+        <v>75</v>
+      </c>
+      <c r="C36" t="s">
+        <v>103</v>
+      </c>
+      <c r="D36" t="s">
+        <v>90</v>
+      </c>
+      <c r="E36" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A37" s="11" t="s">
+        <v>171</v>
+      </c>
+      <c r="B37" t="s">
+        <v>75</v>
+      </c>
+      <c r="C37" t="s">
+        <v>104</v>
+      </c>
+      <c r="D37" t="s">
+        <v>90</v>
+      </c>
+      <c r="E37" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="36" x14ac:dyDescent="0.55000000000000004">
+      <c r="A38" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="B38" t="s">
+        <v>75</v>
+      </c>
+      <c r="C38" t="s">
+        <v>105</v>
+      </c>
+      <c r="D38" t="s">
+        <v>90</v>
+      </c>
+      <c r="E38" s="10" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A39" s="11" t="s">
+        <v>173</v>
+      </c>
+      <c r="B39" t="s">
+        <v>75</v>
+      </c>
+      <c r="C39" t="s">
+        <v>105</v>
+      </c>
+      <c r="D39" t="s">
+        <v>90</v>
+      </c>
+      <c r="E39" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A40" s="11" t="s">
+        <v>174</v>
+      </c>
+      <c r="B40" t="s">
+        <v>134</v>
+      </c>
+      <c r="C40" t="s">
+        <v>76</v>
+      </c>
+      <c r="D40" t="s">
+        <v>79</v>
+      </c>
+      <c r="E40" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="A2" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>